<commit_message>
0.4.1 kiírja a maganut tavot
</commit_message>
<xml_diff>
--- a/2021-01__Teszt_Elek__ELEK-01_gkelsz.xlsx
+++ b/2021-01__Teszt_Elek__ELEK-01_gkelsz.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
   <si>
     <t>ÚTNYILVÁNTARTÁS</t>
   </si>
@@ -131,7 +131,7 @@
     <t>5678</t>
   </si>
   <si>
-    <t>7099</t>
+    <t>10906</t>
   </si>
   <si>
     <t xml:space="preserve"> Teszt Elek</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve"> 16,5</t>
   </si>
   <si>
-    <t>1423</t>
+    <t>5485</t>
   </si>
   <si>
     <t>0.0</t>
@@ -201,6 +201,60 @@
   </si>
   <si>
     <t>AKHB2200/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Szombathely Éhen Gyula tér 2.</t>
+  </si>
+  <si>
+    <t>AKHB2078/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Edelény Antal György u. 3.</t>
+  </si>
+  <si>
+    <t>AKHB2144/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Monostorpályi Landler tér 4.</t>
+  </si>
+  <si>
+    <t>AKHB2122/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Nyírbátor Debreceni út 71.</t>
+  </si>
+  <si>
+    <t>AKHB2317/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Cegléd Ipartelepi u. 3.</t>
+  </si>
+  <si>
+    <t>AKHB2340/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Sárvár Rákóczi u. 83.</t>
+  </si>
+  <si>
+    <t>AKHB2362/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Nyíregyháza Állomás tér 3.</t>
+  </si>
+  <si>
+    <t>AKHB2670/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Budapest Andrássy út 49.</t>
+  </si>
+  <si>
+    <t>AKHK2155/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>Debrecen Füredi út 27.</t>
+  </si>
+  <si>
+    <t>AKHB2072/K &amp; H BANK ZRT.</t>
   </si>
 </sst>
 </file>
@@ -1545,13 +1599,13 @@
       </c>
       <c r="G19" s="25" t="n">
         <f t="shared" si="0"/>
-        <v>7101.0</v>
+        <v>7358.0</v>
       </c>
       <c r="H19" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I19" s="21" t="n">
-        <v>122.0</v>
+        <v>379.0</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>23</v>
@@ -1561,239 +1615,463 @@
       <c r="A20" s="19">
         <v>11</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="25" t="str">
+      <c r="B20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="19"/>
+        <v>7507.0</v>
+      </c>
+      <c r="H20" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I20" s="21" t="n">
+        <v>149.0</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>12</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="25" t="str">
+      <c r="B21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="19"/>
+        <v>7958.0</v>
+      </c>
+      <c r="H21" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I21" s="21" t="n">
+        <v>451.0</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>13</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="25" t="str">
+      <c r="B22" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="19"/>
+        <v>8123.0</v>
+      </c>
+      <c r="H22" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I22" s="21" t="n">
+        <v>165.0</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>14</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="25" t="str">
+      <c r="B23" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="19"/>
+        <v>8196.0</v>
+      </c>
+      <c r="H23" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="21" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>15</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="25" t="str">
+      <c r="B24" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="19"/>
+        <v>8440.0</v>
+      </c>
+      <c r="H24" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I24" s="21" t="n">
+        <v>244.0</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>16</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="25" t="str">
+      <c r="B25" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="19"/>
+        <v>8726.0</v>
+      </c>
+      <c r="H25" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I25" s="21" t="n">
+        <v>286.0</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>17</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="25" t="str">
+      <c r="B26" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="19"/>
+        <v>9187.0</v>
+      </c>
+      <c r="H26" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I26" s="21" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>18</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="25" t="str">
+      <c r="B27" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="19"/>
+        <v>9547.0</v>
+      </c>
+      <c r="H27" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I27" s="21" t="n">
+        <v>360.0</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>19</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="25" t="str">
+      <c r="B28" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="19"/>
+        <v>9649.0</v>
+      </c>
+      <c r="H28" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I28" s="21" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>20</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="25" t="str">
+      <c r="B29" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="19"/>
+        <v>9751.0</v>
+      </c>
+      <c r="H29" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I29" s="21" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>21</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="25" t="str">
+      <c r="B30" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="19"/>
+        <v>10104.0</v>
+      </c>
+      <c r="H30" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I30" s="21" t="n">
+        <v>353.0</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>22</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="25" t="str">
+      <c r="B31" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="19"/>
+        <v>10457.0</v>
+      </c>
+      <c r="H31" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="21" t="n">
+        <v>353.0</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>23</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="25" t="str">
+      <c r="B32" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="19"/>
+        <v>10810.0</v>
+      </c>
+      <c r="H32" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I32" s="21" t="n">
+        <v>353.0</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>24</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="25" t="str">
+      <c r="B33" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="25" t="n">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="19"/>
+        <v>11163.0</v>
+      </c>
+      <c r="H33" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I33" s="21" t="n">
+        <v>353.0</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
@@ -4162,7 +4440,7 @@
       </c>
       <c r="L172" s="34" t="str">
         <f>SUM(I10:I105)</f>
-        <v>1423</v>
+        <v>5485</v>
       </c>
       <c r="M172" s="35"/>
     </row>
@@ -4187,11 +4465,11 @@
       </c>
       <c r="L173" s="37" t="str">
         <f>SUMIF(J10:J105,"M",I10:I105)</f>
-        <v>244</v>
+        <v>501</v>
       </c>
       <c r="M173" s="38" t="str">
         <f>L173/L172</f>
-        <v>17%</v>
+        <v>9.%</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -4215,7 +4493,7 @@
       </c>
       <c r="L174" s="40" t="str">
         <f>C5+L172</f>
-        <v>7099</v>
+        <v>10906</v>
       </c>
       <c r="M174" s="41"/>
     </row>

</xml_diff>